<commit_message>
Added data for recommendation framework
</commit_message>
<xml_diff>
--- a/ChangeData.xlsx
+++ b/ChangeData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33700" yWindow="40" windowWidth="19060" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="52760" yWindow="0" windowWidth="19160" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="130">
   <si>
     <t>JFreeChart</t>
   </si>
@@ -4208,6 +4209,27 @@
  * limitations under the License.
  */</t>
   </si>
+  <si>
+    <t>Total Parameter Object</t>
+  </si>
+  <si>
+    <t>Total Strategy</t>
+  </si>
+  <si>
+    <t>Total Comments</t>
+  </si>
+  <si>
+    <t>Actual Parameter Object</t>
+  </si>
+  <si>
+    <t>Actual Strategy</t>
+  </si>
+  <si>
+    <t>Should Have Comments</t>
+  </si>
+  <si>
+    <t>Should Not have</t>
+  </si>
 </sst>
 </file>
 
@@ -4238,12 +4260,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4255,7 +4283,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4269,26 +4297,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6374,12 +6421,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -6432,11 +6483,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409">
+    <row r="2" spans="1:16" ht="405">
       <c r="A2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -6453,7 +6504,7 @@
       <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -6464,7 +6515,7 @@
       <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -6553,7 +6604,7 @@
       <c r="A8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -6665,39 +6716,39 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="409">
-      <c r="A12" t="s">
+    <row r="12" spans="1:16" s="4" customFormat="1" ht="409">
+      <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="409">
-      <c r="A13" t="s">
+    <row r="13" spans="1:16" s="4" customFormat="1" ht="409">
+      <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="225">
-      <c r="A14" t="s">
+    <row r="14" spans="1:16" s="4" customFormat="1" ht="225">
+      <c r="A14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -6726,14 +6777,14 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="409">
-      <c r="A17" t="s">
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="409">
+      <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>118</v>
       </c>
     </row>
@@ -6815,7 +6866,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="285">
+    <row r="24" spans="1:12" ht="195">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -6837,7 +6888,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="255">
+    <row r="26" spans="1:12" ht="180">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -6857,6 +6908,234 @@
       </c>
       <c r="H27" s="1" t="s">
         <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data for creating the trend graph
</commit_message>
<xml_diff>
--- a/ChangeData.xlsx
+++ b/ChangeData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="52760" yWindow="0" windowWidth="19160" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="130">
   <si>
     <t>JFreeChart</t>
   </si>
@@ -887,50 +887,6 @@
      *
      * @return instance of provider class if found or null
      */</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strategy
-Method Signature
-Comments
-// if that worked, we're on 1.2.
-// ignore it
-/*
- * Copyright 2002-2008 The Apache Software Foundation.
- * 
- * Licensed under the Apache License, Version 2.0 (the "License");
- * you may not use this file except in compliance with the License.
- * You may obtain a copy of the License at
- * 
- *      http://www.apache.org/licenses/LICENSE-2.0
- * 
- * Unless required by applicable law or agreed to in writing, software
- * distributed under the License is distributed on an "AS IS" BASIS,
- * WITHOUT WARRANTIES OR CONDITIONS OF ANY KIND, either express or implied.
- * See the License for the specific language governing permissions and
- * limitations under the License.
- */
-/*
-     * Make this of type Object so that the verifier won't try to
-     * prove its type, thus possibly trying to load the SecuritySupport12
-     * class.
-     */
-/*
-     // don't reference the class explicitly so it doesn't
-     // get dragged in accidentally.
-     c = Class.forName("javax.mail.SecuritySupport12");
-     Constructor cons = c.getConstructor(new Class[] { });
-     ss = (SecuritySupport)cons.newInstance(new Object[] { });
-     */
-/*
-      * Unfortunately, we can't load the class using reflection
-      * because the class is package private.  And the class has
-      * to be package private so the APIs aren't exposed to other
-      * code that could use them to circumvent security.  Thus,
-      * we accept the risk that the direct reference might fail
-      * on some JDK 1.1 JVMs, even though we would never execute
-      * this code in such a case.  Sigh...
-      */
-</t>
   </si>
   <si>
     <t>Strategy
@@ -4230,6 +4186,9 @@
   <si>
     <t>Should Not have</t>
   </si>
+  <si>
+    <t>Blojsom</t>
+  </si>
 </sst>
 </file>
 
@@ -4283,8 +4242,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4317,7 +4300,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4327,6 +4310,18 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4336,11 +4331,516 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00C500"/>
+    </mruColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>JFreeChart</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>_x0012_% Bad Code Quality</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>_x0017_ % Average Code Quality</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>_x0014_ % Good Code Quality</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$16:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>26.49889062008643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.074398755025691</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.96675431959353</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CyberNeko</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>_x0012_% Bad Code Quality</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>_x0017_ % Average Code Quality</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>_x0014_ % Good Code Quality</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$36:$G$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>58.37789987789988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.367521367521367</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.25457875457875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Blojsom</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>_x0012_% Bad Code Quality</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>_x0017_ % Average Code Quality</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>_x0014_ % Good Code Quality</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$50:$G$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64.76962653046183</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.708961336876024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.52141213266214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4665,20 +5165,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A33" sqref="A33"/>
-      <selection pane="topRight" activeCell="A39" sqref="A39:O65"/>
+      <selection pane="topRight" activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
-    <col min="3" max="3" width="51.83203125" customWidth="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -5385,6 +5885,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="16" spans="1:14">
+      <c r="E16">
+        <f>AVERAGE(E2:E15)</f>
+        <v>26.498890620086428</v>
+      </c>
+      <c r="F16">
+        <f>AVERAGE(F2:F15)</f>
+        <v>2.0743987550256913</v>
+      </c>
+      <c r="G16">
+        <f>AVERAGE(G2:G15)</f>
+        <v>64.966754319593534</v>
+      </c>
+    </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>18</v>
@@ -5993,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:14">
       <c r="A33">
         <v>333</v>
       </c>
@@ -6040,7 +6554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:14">
       <c r="A34">
         <v>338</v>
       </c>
@@ -6087,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:14">
       <c r="A35">
         <v>341</v>
       </c>
@@ -6134,279 +6648,621 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
-      <c r="A39" t="s">
+    <row r="36" spans="1:14">
+      <c r="E36">
+        <f>AVERAGE(E21:E35)</f>
+        <v>58.377899877899878</v>
+      </c>
+      <c r="F36">
+        <f>AVERAGE(F21:F35)</f>
+        <v>9.367521367521368</v>
+      </c>
+      <c r="G36">
+        <f>AVERAGE(G21:G35)</f>
+        <v>32.254578754578759</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L38" t="s">
+        <v>38</v>
+      </c>
+      <c r="M38" t="s">
+        <v>39</v>
+      </c>
+      <c r="N38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>2870</v>
+      </c>
+      <c r="B39">
+        <v>2.25</v>
+      </c>
+      <c r="C39">
+        <f>44+18+11+115</f>
+        <v>188</v>
+      </c>
+      <c r="D39">
+        <f>H39+I39+J39+K39+L39+M39+N39</f>
+        <v>159</v>
+      </c>
+      <c r="E39">
+        <f xml:space="preserve"> (H39 + I39 + J39) * 100 / D39</f>
+        <v>44.025157232704402</v>
+      </c>
+      <c r="F39">
+        <f>K39*100/D39</f>
+        <v>6.9182389937106921</v>
+      </c>
+      <c r="G39">
+        <f xml:space="preserve"> (L39 + M39 + N39)*100/D39</f>
+        <v>49.056603773584904</v>
+      </c>
+      <c r="H39">
+        <v>54</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <v>6</v>
+      </c>
+      <c r="K39">
+        <v>11</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>2936</v>
+      </c>
+      <c r="B40">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C40">
+        <f>47+19+11+121</f>
+        <v>198</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:D49" si="6">H40+I40+J40+K40+L40+M40+N40</f>
+        <v>48</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:E49" si="7" xml:space="preserve"> (H40 + I40 + J40) * 100 / D40</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ref="F40:F49" si="8">K40*100/D40</f>
+        <v>6.25</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40:G49" si="9" xml:space="preserve"> (L40 + M40 + N40)*100/D40</f>
+        <v>10.416666666666666</v>
+      </c>
+      <c r="H40">
+        <v>23</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <v>7</v>
+      </c>
+      <c r="K40">
+        <v>3</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>2983</v>
+      </c>
+      <c r="B41">
+        <v>2.27</v>
+      </c>
+      <c r="C41">
+        <f>47+23+11+125</f>
+        <v>206</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="8"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="9"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H41">
+        <v>20</v>
+      </c>
+      <c r="I41">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>3013</v>
+      </c>
+      <c r="B42">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="C42">
+        <f>47+27+11+131</f>
+        <v>216</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="E42">
+        <f t="shared" si="7"/>
+        <v>61.111111111111114</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="9"/>
+        <v>38.888888888888886</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>3073</v>
+      </c>
+      <c r="B43">
+        <v>2.29</v>
+      </c>
+      <c r="C43">
+        <f>49+132+11+26</f>
+        <v>218</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="6"/>
+        <v>181</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="7"/>
+        <v>50.828729281767956</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="8"/>
+        <v>2.7624309392265194</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="9"/>
+        <v>46.408839779005525</v>
+      </c>
+      <c r="H43">
+        <v>78</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="K43">
+        <v>5</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>2</v>
+      </c>
+      <c r="N43">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>3133</v>
+      </c>
+      <c r="B44">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C44">
+        <f>49+138+11+26</f>
+        <v>224</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="H44">
+        <v>13</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>3480</v>
+      </c>
+      <c r="B45">
+        <v>2.31</v>
+      </c>
+      <c r="C45">
+        <f>49+138+11+26</f>
+        <v>224</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="6"/>
+        <v>119</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="7"/>
+        <v>52.941176470588232</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="8"/>
+        <v>3.3613445378151261</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="9"/>
+        <v>43.69747899159664</v>
+      </c>
+      <c r="H45">
+        <v>53</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>3498</v>
+      </c>
+      <c r="B46">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C46">
+        <f>49+26+11+138</f>
+        <v>224</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="7"/>
+        <v>81.818181818181813</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="9"/>
+        <v>18.181818181818183</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47">
+        <v>3530</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <f>46+125+8+30</f>
+        <v>209</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="7"/>
+        <v>92.857142857142861</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="8"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="9"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H47">
         <v>20</v>
       </c>
-      <c r="D39" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" t="s">
-        <v>26</v>
-      </c>
-      <c r="J39" t="s">
-        <v>27</v>
-      </c>
-      <c r="K39" t="s">
-        <v>28</v>
-      </c>
-      <c r="L39" t="s">
-        <v>29</v>
-      </c>
-      <c r="M39" t="s">
-        <v>30</v>
-      </c>
-      <c r="N39" t="s">
-        <v>31</v>
-      </c>
-      <c r="O39" t="s">
-        <v>32</v>
-      </c>
-      <c r="P39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="255">
-      <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="345">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="409">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="409">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="240">
-      <c r="A44" t="s">
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48">
+        <v>3629</v>
+      </c>
+      <c r="B48">
+        <v>3.1</v>
+      </c>
+      <c r="C48">
+        <f>46+30+8+140</f>
+        <v>224</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="6"/>
+        <v>173</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="7"/>
+        <v>39.884393063583815</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="8"/>
+        <v>4.0462427745664744</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="9"/>
+        <v>56.069364161849713</v>
+      </c>
+      <c r="H48">
         <v>48</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="345">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="255">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="409">
-      <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="409">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="I48">
+        <v>12</v>
+      </c>
+      <c r="J48">
+        <v>9</v>
+      </c>
+      <c r="K48">
+        <v>7</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="315">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="409">
-      <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="409">
-      <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="105">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="409">
-      <c r="A53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="409">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="409">
-      <c r="A55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="409">
-      <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="409">
-      <c r="A57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="409">
-      <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="409">
-      <c r="A59" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="360">
-      <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="135">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="120">
-      <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="105">
-      <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="120">
-      <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="90">
-      <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>94</v>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <v>3657</v>
+      </c>
+      <c r="B49">
+        <v>3.2</v>
+      </c>
+      <c r="C49">
+        <f>31+46+8+151</f>
+        <v>236</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="7"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="8"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="9"/>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="H49">
+        <v>8</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="E50">
+        <f>AVERAGE(E39:E49)</f>
+        <v>64.769626530461835</v>
+      </c>
+      <c r="F50">
+        <f>AVERAGE(F39:F49)</f>
+        <v>3.7089613368760244</v>
+      </c>
+      <c r="G50">
+        <f>AVERAGE(G39:G49)</f>
+        <v>31.521412132662135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6419,8 +7275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -6491,13 +7347,13 @@
         <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="409">
@@ -6508,7 +7364,7 @@
         <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="409">
@@ -6525,7 +7381,7 @@
         <v>72</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="409">
@@ -6542,7 +7398,7 @@
         <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>73</v>
@@ -6554,7 +7410,7 @@
         <v>73</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>73</v>
@@ -6597,7 +7453,7 @@
         <v>75</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="409">
@@ -6608,10 +7464,10 @@
         <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="409">
@@ -6622,40 +7478,40 @@
         <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="409">
@@ -6663,46 +7519,46 @@
         <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="409">
@@ -6713,7 +7569,7 @@
         <v>78</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="4" customFormat="1" ht="409">
@@ -6732,10 +7588,10 @@
         <v>55</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="4" customFormat="1" ht="225">
@@ -6743,13 +7599,13 @@
         <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="409">
@@ -6757,13 +7613,13 @@
         <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="409">
@@ -6771,10 +7627,10 @@
         <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="4" customFormat="1" ht="409">
@@ -6782,10 +7638,10 @@
         <v>59</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="409">
@@ -6793,16 +7649,16 @@
         <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="409">
@@ -6810,10 +7666,10 @@
         <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="409">
@@ -6821,13 +7677,13 @@
         <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="409">
@@ -6835,10 +7691,10 @@
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="409">
@@ -6846,10 +7702,10 @@
         <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="285">
@@ -6857,13 +7713,13 @@
         <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="195">
@@ -6871,10 +7727,10 @@
         <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="409">
@@ -6882,10 +7738,10 @@
         <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="180">
@@ -6893,10 +7749,10 @@
         <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="409">
@@ -6904,10 +7760,10 @@
         <v>69</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -6945,25 +7801,25 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>124</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
-      </c>
-      <c r="H1" t="s">
-        <v>129</v>
       </c>
       <c r="I1" t="s">
         <v>26</v>

</xml_diff>